<commit_message>
Modified scripts in to 1PENTITLEMENT
</commit_message>
<xml_diff>
--- a/src/test/test-data/EntitlementsTestData.xlsx
+++ b/src/test/test-data/EntitlementsTestData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="35">
   <si>
     <t>TESTNAME</t>
   </si>
@@ -106,9 +106,6 @@
     <t>/entitlements/3ee9fb20-ba2e-4323-98e5-4b08ace79bc62/entitled</t>
   </si>
   <si>
-    <t>?(entitilement=108902 OR entitilement=215404)</t>
-  </si>
-  <si>
     <t>Verify that to get entitlement details by passing valid entitlement Id</t>
   </si>
   <si>
@@ -119,6 +116,9 @@
   </si>
   <si>
     <t>status=403||errorCode=403.1.1||errorMessage=Entitlement does not exist</t>
+  </si>
+  <si>
+    <t>?entitilement=108902 OR entitilement=215404</t>
   </si>
 </sst>
 </file>
@@ -514,22 +514,22 @@
   <dimension ref="A1:L31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="L2" sqref="L2:L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="46.140625" customWidth="1"/>
-    <col min="3" max="3" width="16" customWidth="1"/>
-    <col min="4" max="4" width="60.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="37.85546875" customWidth="1"/>
-    <col min="7" max="7" width="44.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="54.7109375" customWidth="1"/>
-    <col min="9" max="9" width="18" customWidth="1"/>
-    <col min="10" max="10" width="25.28515625" customWidth="1"/>
-    <col min="11" max="11" width="14.7109375" customWidth="1"/>
-    <col min="12" max="12" width="13" customWidth="1"/>
+    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="46.140625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="60.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="37.85546875" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="44.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="54.7109375" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="18" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="25.28515625" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="14.7109375" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="13" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -591,10 +591,9 @@
       <c r="H2" s="6"/>
       <c r="I2" s="2"/>
       <c r="J2" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K2" s="2"/>
-      <c r="L2" s="1"/>
     </row>
     <row r="3" spans="1:12" ht="45">
       <c r="A3" s="1" t="s">
@@ -617,17 +616,16 @@
       <c r="H3" s="6"/>
       <c r="I3" s="2"/>
       <c r="J3" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K3" s="2"/>
-      <c r="L3" s="1"/>
     </row>
     <row r="4" spans="1:12" ht="30">
       <c r="A4" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>24</v>
@@ -643,10 +641,9 @@
       <c r="H4" s="6"/>
       <c r="I4" s="2"/>
       <c r="J4" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K4" s="2"/>
-      <c r="L4" s="1"/>
     </row>
     <row r="5" spans="1:12" ht="45">
       <c r="A5" s="1" t="s">
@@ -669,12 +666,11 @@
       <c r="H5" s="7"/>
       <c r="I5" s="1"/>
       <c r="J5" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K5" s="1"/>
-      <c r="L5" s="1"/>
-    </row>
-    <row r="6" spans="1:12" ht="30">
+    </row>
+    <row r="6" spans="1:12" ht="45">
       <c r="A6" s="1" t="s">
         <v>20</v>
       </c>
@@ -692,13 +688,14 @@
       </c>
       <c r="F6" s="8"/>
       <c r="G6" s="1" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="H6" s="7"/>
       <c r="I6" s="1"/>
-      <c r="J6" s="6"/>
+      <c r="J6" s="6" t="s">
+        <v>32</v>
+      </c>
       <c r="K6" s="1"/>
-      <c r="L6" s="1"/>
     </row>
     <row r="7" spans="1:12" ht="45">
       <c r="A7" s="1" t="s">
@@ -718,15 +715,14 @@
       </c>
       <c r="F7" s="8"/>
       <c r="G7" s="1" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
       <c r="J7" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K7" s="1"/>
-      <c r="L7" s="1"/>
     </row>
     <row r="8" spans="1:12">
       <c r="A8" s="1"/>
@@ -1066,5 +1062,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added Test cases in EntitlementsTestData
</commit_message>
<xml_diff>
--- a/src/test/test-data/EntitlementsTestData.xlsx
+++ b/src/test/test-data/EntitlementsTestData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="48">
   <si>
     <t>TESTNAME</t>
   </si>
@@ -91,21 +91,12 @@
     <t>1PENTITLEMENTS</t>
   </si>
   <si>
-    <t>/entitlements/3ee9fb20-ba2e-4323-98e5-4b08ace79bc6</t>
-  </si>
-  <si>
-    <t>/entitlements/3ee9fb20-ba2e-4323-98e5-4b08ace79bc62</t>
-  </si>
-  <si>
     <t>/entitlements/entitlement/214504</t>
   </si>
   <si>
     <t>/entitlements/entitlement/2145044</t>
   </si>
   <si>
-    <t>/entitlements/3ee9fb20-ba2e-4323-98e5-4b08ace79bc62/entitled</t>
-  </si>
-  <si>
     <t>Verify that to get entitlement details by passing valid entitlement Id</t>
   </si>
   <si>
@@ -118,7 +109,55 @@
     <t>status=403||errorCode=403.1.1||errorMessage=Entitlement does not exist</t>
   </si>
   <si>
-    <t>?entitilement=108902 OR entitilement=215404</t>
+    <t>/entitlements/(SYS_USER3)/entitled</t>
+  </si>
+  <si>
+    <t>/entitlements/(SYS_USER3)</t>
+  </si>
+  <si>
+    <t>Verify that to get specific entitlement of the user by passing valid truid and valid entitlement name</t>
+  </si>
+  <si>
+    <t>status=200||skus=DRA_TARGET_DRUG||X-1P-ENT=DRA</t>
+  </si>
+  <si>
+    <t>Verify that to get morethan one specific entitlement of the user by passing valid truid and valid entitlement names saperated by comma(,)</t>
+  </si>
+  <si>
+    <t>/entitlements/filter/(SYS_USER3)/DRA_TARGET_DRUG</t>
+  </si>
+  <si>
+    <t>/entitlements/filter/(SYS_USER3)/DRA_TARGET_DRUG,IPA_TEST_SKU</t>
+  </si>
+  <si>
+    <t>status=200||skus=DRA_TARGET_DRUG||skus=IPA_TEST_SKU||X-1P-ENT=DRA</t>
+  </si>
+  <si>
+    <t>/entitlements/(SYS_USER3)1/entitled</t>
+  </si>
+  <si>
+    <t>?entitilement=214504 OR entitilement=215802</t>
+  </si>
+  <si>
+    <t>/entitlements/(SYS_USER3)1</t>
+  </si>
+  <si>
+    <t>status=403||errorCode=403.1.1||errorMessage=User does not have sku</t>
+  </si>
+  <si>
+    <t>OPQA-3852</t>
+  </si>
+  <si>
+    <t>OPQA-3853</t>
+  </si>
+  <si>
+    <t>Verify that to get error status by passing invalid truid and valid entitlement id</t>
+  </si>
+  <si>
+    <t>/entitlements/filter/(SYS_USER3)1/DRA_TARGET_DRUG</t>
+  </si>
+  <si>
+    <t>OPQA-3856</t>
   </si>
 </sst>
 </file>
@@ -514,7 +553,7 @@
   <dimension ref="A1:L31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2:L7"/>
+      <selection activeCell="L10" sqref="L2:L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -522,7 +561,7 @@
     <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="46.140625" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="16" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="60.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="75.28515625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="37.85546875" customWidth="1" collapsed="1"/>
     <col min="7" max="7" width="44.5703125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="8" max="8" width="54.7109375" customWidth="1" collapsed="1"/>
@@ -581,7 +620,7 @@
         <v>24</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>12</v>
@@ -591,7 +630,7 @@
       <c r="H2" s="6"/>
       <c r="I2" s="2"/>
       <c r="J2" s="6" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="K2" s="2"/>
     </row>
@@ -606,7 +645,7 @@
         <v>24</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>12</v>
@@ -616,7 +655,7 @@
       <c r="H3" s="6"/>
       <c r="I3" s="2"/>
       <c r="J3" s="6" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="K3" s="2"/>
     </row>
@@ -625,13 +664,13 @@
         <v>17</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>24</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>12</v>
@@ -641,7 +680,7 @@
       <c r="H4" s="6"/>
       <c r="I4" s="2"/>
       <c r="J4" s="6" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="K4" s="2"/>
     </row>
@@ -656,7 +695,7 @@
         <v>24</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E5" s="8" t="s">
         <v>12</v>
@@ -666,7 +705,7 @@
       <c r="H5" s="7"/>
       <c r="I5" s="1"/>
       <c r="J5" s="6" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="K5" s="1"/>
     </row>
@@ -681,19 +720,19 @@
         <v>24</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E6" s="8" t="s">
         <v>12</v>
       </c>
       <c r="F6" s="8"/>
       <c r="G6" s="1" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="H6" s="7"/>
       <c r="I6" s="1"/>
       <c r="J6" s="6" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="K6" s="1"/>
     </row>
@@ -708,63 +747,96 @@
         <v>24</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="E7" s="8" t="s">
         <v>12</v>
       </c>
       <c r="F7" s="8"/>
       <c r="G7" s="1" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
       <c r="J7" s="6" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="K7" s="1"/>
     </row>
-    <row r="8" spans="1:12">
-      <c r="A8" s="1"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="8"/>
+    <row r="8" spans="1:12" ht="45">
+      <c r="A8" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>12</v>
+      </c>
       <c r="F8" s="1"/>
       <c r="G8" s="7"/>
       <c r="H8" s="7"/>
       <c r="I8" s="1"/>
-      <c r="J8" s="6"/>
+      <c r="J8" s="6" t="s">
+        <v>34</v>
+      </c>
       <c r="K8" s="1"/>
-      <c r="L8" s="1"/>
-    </row>
-    <row r="9" spans="1:12">
-      <c r="A9" s="1"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="8"/>
+    </row>
+    <row r="9" spans="1:12" ht="45">
+      <c r="A9" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>12</v>
+      </c>
       <c r="F9" s="1"/>
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
       <c r="I9" s="1"/>
-      <c r="J9" s="6"/>
+      <c r="J9" s="6" t="s">
+        <v>38</v>
+      </c>
       <c r="K9" s="1"/>
-      <c r="L9" s="1"/>
-    </row>
-    <row r="10" spans="1:12">
-      <c r="A10" s="1"/>
-      <c r="B10" s="7"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="8"/>
+    </row>
+    <row r="10" spans="1:12" ht="45">
+      <c r="A10" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>12</v>
+      </c>
       <c r="F10" s="1"/>
       <c r="G10" s="7"/>
       <c r="H10" s="7"/>
       <c r="I10" s="1"/>
-      <c r="J10" s="6"/>
+      <c r="J10" s="6" t="s">
+        <v>29</v>
+      </c>
       <c r="K10" s="1"/>
-      <c r="L10" s="1"/>
     </row>
     <row r="11" spans="1:12">
       <c r="A11" s="1"/>

</xml_diff>

<commit_message>
Modified validations in Entitlement.xlsx file
</commit_message>
<xml_diff>
--- a/src/test/test-data/EntitlementsTestData.xlsx
+++ b/src/test/test-data/EntitlementsTestData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="49">
   <si>
     <t>TESTNAME</t>
   </si>
@@ -158,6 +158,9 @@
   </si>
   <si>
     <t>OPQA-3856</t>
+  </si>
+  <si>
+    <t>status=200||trialSkus=DRA_TARGET_DRUG</t>
   </si>
 </sst>
 </file>
@@ -553,7 +556,7 @@
   <dimension ref="A1:L31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="L10" sqref="L2:L10"/>
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -680,7 +683,7 @@
       <c r="H4" s="6"/>
       <c r="I4" s="2"/>
       <c r="J4" s="6" t="s">
-        <v>28</v>
+        <v>48</v>
       </c>
       <c r="K4" s="2"/>
     </row>

</xml_diff>

<commit_message>
New test case added to entitlements
</commit_message>
<xml_diff>
--- a/src/test/test-data/EntitlementsTestData.xlsx
+++ b/src/test/test-data/EntitlementsTestData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="52">
   <si>
     <t>TESTNAME</t>
   </si>
@@ -161,6 +161,15 @@
   </si>
   <si>
     <t>status=200||trialSkus=DRA_TARGET_DRUG</t>
+  </si>
+  <si>
+    <t>Verify that to get error status by passing valid truid and without entitlements</t>
+  </si>
+  <si>
+    <t>/entitlements/(SYS_USER5)</t>
+  </si>
+  <si>
+    <t>OPQA-5644</t>
   </si>
 </sst>
 </file>
@@ -556,7 +565,7 @@
   <dimension ref="A1:L31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -636,6 +645,7 @@
         <v>28</v>
       </c>
       <c r="K2" s="2"/>
+      <c r="L2" s="1"/>
     </row>
     <row r="3" spans="1:12" ht="45">
       <c r="A3" s="1" t="s">
@@ -841,19 +851,30 @@
       </c>
       <c r="K10" s="1"/>
     </row>
-    <row r="11" spans="1:12">
-      <c r="A11" s="1"/>
-      <c r="B11" s="7"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="8"/>
+    <row r="11" spans="1:12" ht="45">
+      <c r="A11" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>12</v>
+      </c>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
-      <c r="J11" s="7"/>
+      <c r="J11" s="7" t="s">
+        <v>42</v>
+      </c>
       <c r="K11" s="1"/>
-      <c r="L11" s="1"/>
     </row>
     <row r="12" spans="1:12">
       <c r="A12" s="1"/>

</xml_diff>

<commit_message>
Added new testcases for entitlements API
</commit_message>
<xml_diff>
--- a/src/test/test-data/EntitlementsTestData.xlsx
+++ b/src/test/test-data/EntitlementsTestData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="60">
   <si>
     <t>TESTNAME</t>
   </si>
@@ -100,9 +100,6 @@
     <t>Verify that to get entitlement details by passing valid entitlement Id</t>
   </si>
   <si>
-    <t>status=200||skus=DRA_TARGET_DRUG</t>
-  </si>
-  <si>
     <t>status=403||errorCode=403.1.8||errorMessage=Unknowen user</t>
   </si>
   <si>
@@ -170,13 +167,40 @@
   </si>
   <si>
     <t>OPQA-5644</t>
+  </si>
+  <si>
+    <t>status=200||skus=DRA_TARGET_DRUG||skus=DRA_DRUG_DESIGN||skus=IPA_TEST_SKU]||has_trial_skus=true||X-1P-ENT=DRA,IPA</t>
+  </si>
+  <si>
+    <t>errorCode=403.1.5||errorMessage=User have a trial sku</t>
+  </si>
+  <si>
+    <t>/entitlements/(SYS_USER4)/DRA_TARGET_DRUG</t>
+  </si>
+  <si>
+    <t>/entitlements/user/DRA_TARGET_DRUG</t>
+  </si>
+  <si>
+    <t>X-1P-User=(SYS_USER2)</t>
+  </si>
+  <si>
+    <t>OPQA-5649</t>
+  </si>
+  <si>
+    <t>Verify that to get error status and message by passing valid truid and entitlement name for user having trail entitlement</t>
+  </si>
+  <si>
+    <t>OPQA-5650</t>
+  </si>
+  <si>
+    <t>Verify that user is able to get the entitlements list by passing specific entitlement name</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -198,6 +222,19 @@
       <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -245,7 +282,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -267,6 +304,11 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -565,7 +607,7 @@
   <dimension ref="A1:L31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="L2" sqref="L2:L23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -621,7 +663,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="30">
+    <row r="2" spans="1:12" ht="75">
       <c r="A2" s="1" t="s">
         <v>13</v>
       </c>
@@ -632,7 +674,7 @@
         <v>24</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>12</v>
@@ -642,10 +684,9 @@
       <c r="H2" s="6"/>
       <c r="I2" s="2"/>
       <c r="J2" s="6" t="s">
-        <v>28</v>
+        <v>51</v>
       </c>
       <c r="K2" s="2"/>
-      <c r="L2" s="1"/>
     </row>
     <row r="3" spans="1:12" ht="45">
       <c r="A3" s="1" t="s">
@@ -658,7 +699,7 @@
         <v>24</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>12</v>
@@ -668,7 +709,7 @@
       <c r="H3" s="6"/>
       <c r="I3" s="2"/>
       <c r="J3" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K3" s="2"/>
     </row>
@@ -693,7 +734,7 @@
       <c r="H4" s="6"/>
       <c r="I4" s="2"/>
       <c r="J4" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K4" s="2"/>
     </row>
@@ -718,7 +759,7 @@
       <c r="H5" s="7"/>
       <c r="I5" s="1"/>
       <c r="J5" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K5" s="1"/>
     </row>
@@ -733,19 +774,19 @@
         <v>24</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E6" s="8" t="s">
         <v>12</v>
       </c>
       <c r="F6" s="8"/>
       <c r="G6" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H6" s="7"/>
       <c r="I6" s="1"/>
       <c r="J6" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K6" s="1"/>
     </row>
@@ -760,34 +801,34 @@
         <v>24</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E7" s="8" t="s">
         <v>12</v>
       </c>
       <c r="F7" s="8"/>
       <c r="G7" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
       <c r="J7" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K7" s="1"/>
     </row>
     <row r="8" spans="1:12" ht="45">
       <c r="A8" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>24</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E8" s="8" t="s">
         <v>12</v>
@@ -797,22 +838,22 @@
       <c r="H8" s="7"/>
       <c r="I8" s="1"/>
       <c r="J8" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K8" s="1"/>
     </row>
     <row r="9" spans="1:12" ht="45">
       <c r="A9" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>24</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E9" s="8" t="s">
         <v>12</v>
@@ -822,22 +863,22 @@
       <c r="H9" s="7"/>
       <c r="I9" s="1"/>
       <c r="J9" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K9" s="1"/>
     </row>
     <row r="10" spans="1:12" ht="45">
       <c r="A10" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>24</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E10" s="8" t="s">
         <v>12</v>
@@ -847,22 +888,22 @@
       <c r="H10" s="7"/>
       <c r="I10" s="1"/>
       <c r="J10" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K10" s="1"/>
     </row>
     <row r="11" spans="1:12" ht="45">
       <c r="A11" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>24</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E11" s="8" t="s">
         <v>12</v>
@@ -872,35 +913,61 @@
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
       <c r="J11" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K11" s="1"/>
     </row>
-    <row r="12" spans="1:12">
-      <c r="A12" s="1"/>
-      <c r="B12" s="7"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="8"/>
+    <row r="12" spans="1:12" ht="45">
+      <c r="A12" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>12</v>
+      </c>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
-      <c r="J12" s="7"/>
+      <c r="J12" s="12" t="s">
+        <v>52</v>
+      </c>
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
     </row>
-    <row r="13" spans="1:12">
-      <c r="A13" s="1"/>
-      <c r="B13" s="7"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="1"/>
+    <row r="13" spans="1:12" ht="75">
+      <c r="A13" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="F13" s="11" t="s">
+        <v>55</v>
+      </c>
       <c r="G13" s="1"/>
       <c r="H13" s="7"/>
       <c r="I13" s="1"/>
-      <c r="J13" s="7"/>
+      <c r="J13" s="7" t="s">
+        <v>51</v>
+      </c>
       <c r="K13" s="1"/>
       <c r="L13" s="1"/>
     </row>

</xml_diff>

<commit_message>
changes validations for few test cases for entitlements
</commit_message>
<xml_diff>
--- a/src/test/test-data/EntitlementsTestData.xlsx
+++ b/src/test/test-data/EntitlementsTestData.xlsx
@@ -100,9 +100,6 @@
     <t>Verify that to get entitlement details by passing valid entitlement Id</t>
   </si>
   <si>
-    <t>status=403||errorCode=403.1.8||errorMessage=Unknowen user</t>
-  </si>
-  <si>
     <t>status=403||errorCode=403.1.1||errorMessage=Entitlement does not exist</t>
   </si>
   <si>
@@ -194,6 +191,9 @@
   </si>
   <si>
     <t>Verify that user is able to get the entitlements list by passing specific entitlement name</t>
+  </si>
+  <si>
+    <t>status=403||errorCode=403.1.8||errorMessage=Unknown user</t>
   </si>
 </sst>
 </file>
@@ -607,7 +607,7 @@
   <dimension ref="A1:L31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2:L23"/>
+      <selection activeCell="K10" sqref="J10:K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -674,7 +674,7 @@
         <v>24</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>12</v>
@@ -684,7 +684,7 @@
       <c r="H2" s="6"/>
       <c r="I2" s="2"/>
       <c r="J2" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K2" s="2"/>
     </row>
@@ -699,7 +699,7 @@
         <v>24</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>12</v>
@@ -709,7 +709,7 @@
       <c r="H3" s="6"/>
       <c r="I3" s="2"/>
       <c r="J3" s="6" t="s">
-        <v>28</v>
+        <v>59</v>
       </c>
       <c r="K3" s="2"/>
     </row>
@@ -734,7 +734,7 @@
       <c r="H4" s="6"/>
       <c r="I4" s="2"/>
       <c r="J4" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K4" s="2"/>
     </row>
@@ -759,7 +759,7 @@
       <c r="H5" s="7"/>
       <c r="I5" s="1"/>
       <c r="J5" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K5" s="1"/>
     </row>
@@ -774,19 +774,19 @@
         <v>24</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E6" s="8" t="s">
         <v>12</v>
       </c>
       <c r="F6" s="8"/>
       <c r="G6" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H6" s="7"/>
       <c r="I6" s="1"/>
       <c r="J6" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K6" s="1"/>
     </row>
@@ -801,34 +801,34 @@
         <v>24</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E7" s="8" t="s">
         <v>12</v>
       </c>
       <c r="F7" s="8"/>
       <c r="G7" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
       <c r="J7" s="6" t="s">
-        <v>28</v>
+        <v>59</v>
       </c>
       <c r="K7" s="1"/>
     </row>
     <row r="8" spans="1:12" ht="45">
       <c r="A8" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>24</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E8" s="8" t="s">
         <v>12</v>
@@ -838,22 +838,22 @@
       <c r="H8" s="7"/>
       <c r="I8" s="1"/>
       <c r="J8" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K8" s="1"/>
     </row>
     <row r="9" spans="1:12" ht="45">
       <c r="A9" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>24</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E9" s="8" t="s">
         <v>12</v>
@@ -863,22 +863,22 @@
       <c r="H9" s="7"/>
       <c r="I9" s="1"/>
       <c r="J9" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K9" s="1"/>
     </row>
     <row r="10" spans="1:12" ht="45">
       <c r="A10" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>24</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E10" s="8" t="s">
         <v>12</v>
@@ -888,22 +888,22 @@
       <c r="H10" s="7"/>
       <c r="I10" s="1"/>
       <c r="J10" s="6" t="s">
-        <v>28</v>
+        <v>59</v>
       </c>
       <c r="K10" s="1"/>
     </row>
     <row r="11" spans="1:12" ht="45">
       <c r="A11" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>24</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E11" s="8" t="s">
         <v>12</v>
@@ -913,22 +913,22 @@
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
       <c r="J11" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K11" s="1"/>
     </row>
     <row r="12" spans="1:12" ht="45">
       <c r="A12" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B12" s="13" t="s">
         <v>56</v>
-      </c>
-      <c r="B12" s="13" t="s">
-        <v>57</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>24</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E12" s="8" t="s">
         <v>12</v>
@@ -938,35 +938,34 @@
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
       <c r="J12" s="12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="K12" s="1"/>
-      <c r="L12" s="1"/>
     </row>
     <row r="13" spans="1:12" ht="75">
       <c r="A13" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B13" s="7" t="s">
         <v>58</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>59</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>24</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E13" s="8" t="s">
         <v>12</v>
       </c>
       <c r="F13" s="11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G13" s="1"/>
       <c r="H13" s="7"/>
       <c r="I13" s="1"/>
       <c r="J13" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K13" s="1"/>
       <c r="L13" s="1"/>

</xml_diff>

<commit_message>
changes done for entitlements
</commit_message>
<xml_diff>
--- a/src/test/test-data/EntitlementsTestData.xlsx
+++ b/src/test/test-data/EntitlementsTestData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="61">
   <si>
     <t>TESTNAME</t>
   </si>
@@ -194,6 +194,9 @@
   </si>
   <si>
     <t>status=403||errorCode=403.1.8||errorMessage=Unknown user</t>
+  </si>
+  <si>
+    <t>status=200</t>
   </si>
 </sst>
 </file>
@@ -606,8 +609,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="K10" sqref="J10:K11"/>
+    <sheetView tabSelected="1" topLeftCell="E4" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -942,7 +945,7 @@
       </c>
       <c r="K12" s="1"/>
     </row>
-    <row r="13" spans="1:12" ht="75">
+    <row r="13" spans="1:12" ht="30">
       <c r="A13" s="1" t="s">
         <v>57</v>
       </c>
@@ -965,7 +968,7 @@
       <c r="H13" s="7"/>
       <c r="I13" s="1"/>
       <c r="J13" s="7" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="K13" s="1"/>
       <c r="L13" s="1"/>

</xml_diff>

<commit_message>
users are changed for entitlements api
</commit_message>
<xml_diff>
--- a/src/test/test-data/EntitlementsTestData.xlsx
+++ b/src/test/test-data/EntitlementsTestData.xlsx
@@ -172,15 +172,9 @@
     <t>errorCode=403.1.5||errorMessage=User have a trial sku</t>
   </si>
   <si>
-    <t>/entitlements/(SYS_USER4)/DRA_TARGET_DRUG</t>
-  </si>
-  <si>
     <t>/entitlements/user/DRA_TARGET_DRUG</t>
   </si>
   <si>
-    <t>X-1P-User=(SYS_USER2)</t>
-  </si>
-  <si>
     <t>OPQA-5649</t>
   </si>
   <si>
@@ -197,6 +191,12 @@
   </si>
   <si>
     <t>status=200</t>
+  </si>
+  <si>
+    <t>X-1P-User=(SYS_USER4)</t>
+  </si>
+  <si>
+    <t>/entitlements/(SYS_USER2)/DRA_TARGET_DRUG</t>
   </si>
 </sst>
 </file>
@@ -609,8 +609,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E4" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -712,7 +712,7 @@
       <c r="H3" s="6"/>
       <c r="I3" s="2"/>
       <c r="J3" s="6" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="K3" s="2"/>
     </row>
@@ -816,7 +816,7 @@
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
       <c r="J7" s="6" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="K7" s="1"/>
     </row>
@@ -891,7 +891,7 @@
       <c r="H10" s="7"/>
       <c r="I10" s="1"/>
       <c r="J10" s="6" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="K10" s="1"/>
     </row>
@@ -922,16 +922,16 @@
     </row>
     <row r="12" spans="1:12" ht="45">
       <c r="A12" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>24</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="E12" s="8" t="s">
         <v>12</v>
@@ -947,28 +947,28 @@
     </row>
     <row r="13" spans="1:12" ht="30">
       <c r="A13" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>24</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E13" s="8" t="s">
         <v>12</v>
       </c>
       <c r="F13" s="11" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="G13" s="1"/>
       <c r="H13" s="7"/>
       <c r="I13" s="1"/>
       <c r="J13" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="K13" s="1"/>
       <c r="L13" s="1"/>

</xml_diff>

<commit_message>
modifications done in entitlements api
</commit_message>
<xml_diff>
--- a/src/test/test-data/EntitlementsTestData.xlsx
+++ b/src/test/test-data/EntitlementsTestData.xlsx
@@ -196,7 +196,7 @@
     <t>X-1P-User=(SYS_USER4)</t>
   </si>
   <si>
-    <t>/entitlements/(SYS_USER2)/DRA_TARGET_DRUG</t>
+    <t>/entitlements/(SYS_USER2)/IPA_TEST_SKU</t>
   </si>
 </sst>
 </file>
@@ -610,7 +610,7 @@
   <dimension ref="A1:L31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
added new test cases to entitlements
</commit_message>
<xml_diff>
--- a/src/test/test-data/EntitlementsTestData.xlsx
+++ b/src/test/test-data/EntitlementsTestData.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bg00483545\git\1p-api-automation\src\test\test-data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="135" windowWidth="23955" windowHeight="9780"/>
   </bookViews>
@@ -14,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="68">
   <si>
     <t>TESTNAME</t>
   </si>
@@ -197,13 +202,34 @@
   </si>
   <si>
     <t>/entitlements/(SYS_USER2)/IPA_TEST_SKU</t>
+  </si>
+  <si>
+    <t>OPQA-5733</t>
+  </si>
+  <si>
+    <t>/entitlements/2bd6b996-150e-4b1e-a5c4-c3789237c89b</t>
+  </si>
+  <si>
+    <t>status=200|| skus=CMC_CIS_04||skus= CMC_AM||skus= CMC_KG||skus= CMC_GE||skus= CMC_TJ||trial_skus=CMC_CIS_04||trial_skus= CMC_AM||trial_skus= CMC_KG||trial_skus= CMC_GE||trial_skus= CMC_TJ||has_trial_skus=true||X-1P-ENT=CMC</t>
+  </si>
+  <si>
+    <t>Verify that trai skus status value  if user associate with non trail entitlements by passing truid</t>
+  </si>
+  <si>
+    <t>OPQA-5734</t>
+  </si>
+  <si>
+    <t>/entitlements/40541757-5531-4006-bbe7-a46ac7ae2d65</t>
+  </si>
+  <si>
+    <t>status=200|| has_trial_skus=false||X-1P-ENT=CMC</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -285,7 +311,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -312,6 +338,15 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -319,6 +354,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -365,7 +408,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -397,9 +440,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -431,6 +475,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -606,14 +651,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2:L19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="46.140625" customWidth="1" collapsed="1"/>
@@ -628,7 +673,7 @@
     <col min="12" max="12" width="13" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -666,7 +711,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="75">
+    <row r="2" spans="1:12" ht="75" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>13</v>
       </c>
@@ -691,7 +736,7 @@
       </c>
       <c r="K2" s="2"/>
     </row>
-    <row r="3" spans="1:12" ht="45">
+    <row r="3" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>15</v>
       </c>
@@ -716,7 +761,7 @@
       </c>
       <c r="K3" s="2"/>
     </row>
-    <row r="4" spans="1:12" ht="30">
+    <row r="4" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>17</v>
       </c>
@@ -741,7 +786,7 @@
       </c>
       <c r="K4" s="2"/>
     </row>
-    <row r="5" spans="1:12" ht="45">
+    <row r="5" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>18</v>
       </c>
@@ -766,7 +811,7 @@
       </c>
       <c r="K5" s="1"/>
     </row>
-    <row r="6" spans="1:12" ht="45">
+    <row r="6" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>20</v>
       </c>
@@ -793,7 +838,7 @@
       </c>
       <c r="K6" s="1"/>
     </row>
-    <row r="7" spans="1:12" ht="45">
+    <row r="7" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>22</v>
       </c>
@@ -820,7 +865,7 @@
       </c>
       <c r="K7" s="1"/>
     </row>
-    <row r="8" spans="1:12" ht="45">
+    <row r="8" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>41</v>
       </c>
@@ -845,7 +890,7 @@
       </c>
       <c r="K8" s="1"/>
     </row>
-    <row r="9" spans="1:12" ht="45">
+    <row r="9" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>42</v>
       </c>
@@ -870,7 +915,7 @@
       </c>
       <c r="K9" s="1"/>
     </row>
-    <row r="10" spans="1:12" ht="45">
+    <row r="10" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>45</v>
       </c>
@@ -895,7 +940,7 @@
       </c>
       <c r="K10" s="1"/>
     </row>
-    <row r="11" spans="1:12" ht="45">
+    <row r="11" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>49</v>
       </c>
@@ -920,7 +965,7 @@
       </c>
       <c r="K11" s="1"/>
     </row>
-    <row r="12" spans="1:12" ht="45">
+    <row r="12" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>53</v>
       </c>
@@ -945,7 +990,7 @@
       </c>
       <c r="K12" s="1"/>
     </row>
-    <row r="13" spans="1:12" ht="30">
+    <row r="13" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>55</v>
       </c>
@@ -971,37 +1016,59 @@
         <v>58</v>
       </c>
       <c r="K13" s="1"/>
-      <c r="L13" s="1"/>
-    </row>
-    <row r="14" spans="1:12">
-      <c r="A14" s="1"/>
-      <c r="B14" s="7"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="7"/>
-      <c r="I14" s="1"/>
-      <c r="J14" s="7"/>
-      <c r="K14" s="1"/>
-      <c r="L14" s="1"/>
-    </row>
-    <row r="15" spans="1:12">
-      <c r="A15" s="1"/>
-      <c r="B15" s="7"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
-      <c r="J15" s="7"/>
-      <c r="K15" s="1"/>
-      <c r="L15" s="1"/>
-    </row>
-    <row r="16" spans="1:12">
+    </row>
+    <row r="14" spans="1:12" ht="180" x14ac:dyDescent="0.25">
+      <c r="A14" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="D14" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="E14" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="F14" s="17"/>
+      <c r="G14" s="18"/>
+      <c r="H14" s="15"/>
+      <c r="I14" s="14"/>
+      <c r="J14" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="K14" s="14"/>
+      <c r="L14" s="14"/>
+    </row>
+    <row r="15" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A15" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="C15" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="E15" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="F15" s="17"/>
+      <c r="G15" s="18"/>
+      <c r="H15" s="15"/>
+      <c r="I15" s="14"/>
+      <c r="J15" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="K15" s="14"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="7"/>
       <c r="C16" s="1"/>
@@ -1015,7 +1082,7 @@
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
     </row>
-    <row r="17" spans="1:12">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="7"/>
       <c r="C17" s="1"/>
@@ -1029,7 +1096,7 @@
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
     </row>
-    <row r="18" spans="1:12">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="7"/>
       <c r="C18" s="1"/>
@@ -1043,7 +1110,7 @@
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
     </row>
-    <row r="19" spans="1:12">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="7"/>
       <c r="C19" s="1"/>
@@ -1057,7 +1124,7 @@
       <c r="K19" s="1"/>
       <c r="L19" s="1"/>
     </row>
-    <row r="20" spans="1:12">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="7"/>
       <c r="C20" s="1"/>
@@ -1071,7 +1138,7 @@
       <c r="K20" s="1"/>
       <c r="L20" s="1"/>
     </row>
-    <row r="21" spans="1:12">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="7"/>
       <c r="C21" s="1"/>
@@ -1085,7 +1152,7 @@
       <c r="K21" s="1"/>
       <c r="L21" s="1"/>
     </row>
-    <row r="22" spans="1:12">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="7"/>
       <c r="C22" s="1"/>
@@ -1099,7 +1166,7 @@
       <c r="K22" s="1"/>
       <c r="L22" s="1"/>
     </row>
-    <row r="23" spans="1:12">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="7"/>
       <c r="C23" s="1"/>
@@ -1113,7 +1180,7 @@
       <c r="K23" s="1"/>
       <c r="L23" s="1"/>
     </row>
-    <row r="24" spans="1:12">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="7"/>
       <c r="C24" s="1"/>
@@ -1127,7 +1194,7 @@
       <c r="K24" s="1"/>
       <c r="L24" s="1"/>
     </row>
-    <row r="25" spans="1:12">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="7"/>
       <c r="C25" s="1"/>
@@ -1141,7 +1208,7 @@
       <c r="K25" s="1"/>
       <c r="L25" s="1"/>
     </row>
-    <row r="26" spans="1:12">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="7"/>
       <c r="C26" s="1"/>
@@ -1155,7 +1222,7 @@
       <c r="K26" s="1"/>
       <c r="L26" s="1"/>
     </row>
-    <row r="27" spans="1:12">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="7"/>
       <c r="C27" s="1"/>
@@ -1169,7 +1236,7 @@
       <c r="K27" s="1"/>
       <c r="L27" s="1"/>
     </row>
-    <row r="28" spans="1:12">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="7"/>
       <c r="C28" s="1"/>
@@ -1183,7 +1250,7 @@
       <c r="K28" s="1"/>
       <c r="L28" s="1"/>
     </row>
-    <row r="29" spans="1:12">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="7"/>
       <c r="C29" s="1"/>
@@ -1197,7 +1264,7 @@
       <c r="K29" s="7"/>
       <c r="L29" s="1"/>
     </row>
-    <row r="30" spans="1:12">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="7"/>
       <c r="C30" s="1"/>
@@ -1211,7 +1278,7 @@
       <c r="K30" s="1"/>
       <c r="L30" s="1"/>
     </row>
-    <row r="31" spans="1:12">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="7"/>
       <c r="C31" s="1"/>

</xml_diff>